<commit_message>
Yiel for expected && for actual
</commit_message>
<xml_diff>
--- a/Program-5/1.-Planeación/Tool for yield.xlsx
+++ b/Program-5/1.-Planeación/Tool for yield.xlsx
@@ -5,15 +5,16 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardosanzb/Documents/psp-upaep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardosanzb/Documents/psp-upaep/Program-5/1.-Planeación/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="22300" windowHeight="14760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Yield" sheetId="1" r:id="rId1"/>
-    <sheet name="ToDate%" sheetId="2" r:id="rId2"/>
+    <sheet name="Yield Est" sheetId="3" r:id="rId1"/>
+    <sheet name="Yield Act" sheetId="1" r:id="rId2"/>
+    <sheet name="ToDate%" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>FASE</t>
   </si>
@@ -114,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -241,12 +242,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +298,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +582,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A11" sqref="A11:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,9 +813,243 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>4</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f>B2</f>
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <f>C2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2-E2</f>
+        <v>4</v>
+      </c>
+      <c r="G2" s="7">
+        <f>C2+F2</f>
+        <v>4</v>
+      </c>
+      <c r="H2" s="10">
+        <f>(C2/G2)*100</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <f>D2+B3</f>
+        <v>4</v>
+      </c>
+      <c r="E3" s="3">
+        <f>C3+E2</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F6" si="0">D3-E3</f>
+        <v>4</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G7" si="1">C3+F3</f>
+        <v>4</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" ref="H3:H7" si="2">(C3/G3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D7" si="3">D3+B4</f>
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E7" si="4">C4+E3</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="2"/>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="2"/>
+        <v>30.76923076923077</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="2"/>
+        <v>77.777777777777786</v>
+      </c>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7-E7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -883,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="14">
-        <f t="shared" ref="B2:B9" si="1">A9/$A$9</f>
+        <f t="shared" ref="B9" si="1">A9/$A$9</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>